<commit_message>
Got graphics working for Board (walkway, rooms, doors, etc)
</commit_message>
<xml_diff>
--- a/ClueLayoutUpdated.xlsx
+++ b/ClueLayoutUpdated.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quinn\eclipse-workspace\ClueGame\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFA2300-79AE-40C6-9E9D-EE9E0B31663F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{62A22F7E-D4FA-4FF7-ADAB-CF12D0EE9599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{17597C92-5A73-493F-A498-1F3B3F438DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="42">
   <si>
     <t>Number of Doors: 12</t>
   </si>
@@ -157,6 +152,9 @@
   </si>
   <si>
     <t>D*</t>
+  </si>
+  <si>
+    <t>A*</t>
   </si>
 </sst>
 </file>
@@ -640,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFEC89F6-B891-4E34-BD84-9CC01E41E9E5}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1105,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="U6" s="21" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="V6" s="4" t="s">
         <v>6</v>
@@ -1392,11 +1390,11 @@
       <c r="J10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>18</v>
@@ -2141,8 +2139,8 @@
       <c r="C20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>29</v>
+      <c r="D20" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>29</v>
@@ -2224,8 +2222,8 @@
       <c r="E21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>30</v>
+      <c r="F21" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>29</v>
@@ -2266,14 +2264,14 @@
       <c r="S21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="T21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>4</v>
+      <c r="T21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="W21" s="4" t="s">
         <v>28</v>
@@ -2343,14 +2341,14 @@
       <c r="S22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="T22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V22" s="2" t="s">
-        <v>4</v>
+      <c r="T22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="W22" s="4" t="s">
         <v>28</v>
@@ -2663,8 +2661,8 @@
       <c r="W26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X26" s="8" t="s">
-        <v>33</v>
+      <c r="X26" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="Y26" s="4" t="s">
         <v>28</v>

</xml_diff>